<commit_message>
Updated the lab3 assignment
Put back in publishing to Azure, took out validation.
</commit_message>
<xml_diff>
--- a/Labs/Lab01/Lab1Rubric_CS295N.xlsx
+++ b/Labs/Lab01/Lab1Rubric_CS295N.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CS295N-CourseMaterials/Labs/Lab01/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABB3C250-472D-EB43-ACD0-56562F72874E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0535D783-BDD7-6D49-9350-7EF9CEDA0C32}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1860" windowWidth="20420" windowHeight="13460" xr2:uid="{E89A4641-8758-0A47-BBA8-AF46CE147EE8}"/>
+    <workbookView xWindow="5180" yWindow="1720" windowWidth="20420" windowHeight="13460" activeTab="1" xr2:uid="{E89A4641-8758-0A47-BBA8-AF46CE147EE8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Rubric" sheetId="1" r:id="rId1"/>
+    <sheet name="Grade" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
   <si>
     <t>Lab 1</t>
   </si>
@@ -33,15 +34,9 @@
     <t>Excellent work! Everything looks great.</t>
   </si>
   <si>
-    <t>Working MVC site</t>
-  </si>
-  <si>
     <t>GitHub repository</t>
   </si>
   <si>
-    <t>Modifications to the view</t>
-  </si>
-  <si>
     <t>.gitignore</t>
   </si>
   <si>
@@ -64,13 +59,25 @@
   </si>
   <si>
     <t>Requirements</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>main branch</t>
+  </si>
+  <si>
+    <t>Project builds and runs</t>
+  </si>
+  <si>
+    <t>MVC site</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -88,6 +95,14 @@
     </font>
     <font>
       <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -115,10 +130,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,15 +449,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{281C4FE9-3D20-9541-ADFE-932BAB85A5E5}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.1640625" customWidth="1"/>
+    <col min="1" max="1" width="25.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -449,69 +465,230 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15">
+        <f>SUM(B4:B13)</f>
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4A17B91-A5F8-5746-983D-59BEC50C3108}">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
-        <v>11</v>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>10</v>
+      <c r="C5">
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8">
-        <v>10</v>
-      </c>
+      <c r="A8" s="2"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>5</v>
+      <c r="A9" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="1">
+        <f>SUM(B4:B13)</f>
+        <v>50</v>
+      </c>
+      <c r="C15" s="1">
+        <f>SUM(C4:C13)</f>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the notes and lab assignment
</commit_message>
<xml_diff>
--- a/Labs/Lab01/Lab1Rubric_CS295N.xlsx
+++ b/Labs/Lab01/Lab1Rubric_CS295N.xlsx
@@ -1,32 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CS295N-CourseMaterials/Labs/Lab01/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\CS295N-CourseMaterials\Labs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0535D783-BDD7-6D49-9350-7EF9CEDA0C32}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E140BDFD-2776-40F5-861C-B4534FEA6101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1720" windowWidth="20420" windowHeight="13460" activeTab="1" xr2:uid="{E89A4641-8758-0A47-BBA8-AF46CE147EE8}"/>
+    <workbookView xWindow="22716" yWindow="2052" windowWidth="7932" windowHeight="14148" xr2:uid="{E89A4641-8758-0A47-BBA8-AF46CE147EE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="1" r:id="rId1"/>
     <sheet name="Grade" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
   <si>
     <t>Lab 1</t>
   </si>
@@ -71,6 +82,9 @@
   </si>
   <si>
     <t>MVC site</t>
+  </si>
+  <si>
+    <t>Correct .NET Version</t>
   </si>
 </sst>
 </file>
@@ -449,23 +463,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{281C4FE9-3D20-9541-ADFE-932BAB85A5E5}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.1640625" customWidth="1"/>
+    <col min="1" max="1" width="25.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -474,12 +488,12 @@
       </c>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -487,7 +501,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -495,7 +509,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -503,52 +517,60 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B10">
+      <c r="B11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="B14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B15">
-        <f>SUM(B4:B13)</f>
+      <c r="B16" s="1">
+        <f>SUM(B4:B14)</f>
         <v>50</v>
       </c>
     </row>
@@ -559,25 +581,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4A17B91-A5F8-5746-983D-59BEC50C3108}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.8984375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -588,12 +613,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -604,7 +629,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -615,7 +640,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -626,72 +651,84 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B10">
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11">
-        <v>5</v>
-      </c>
-      <c r="C11">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12">
-        <v>5</v>
-      </c>
-      <c r="C12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13">
-        <v>5</v>
-      </c>
-      <c r="C13">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="1">
-        <f>SUM(B4:B13)</f>
+      <c r="B16" s="1">
+        <f>SUM(B4:B14)</f>
         <v>50</v>
       </c>
-      <c r="C15" s="1">
-        <f>SUM(C4:C13)</f>
+      <c r="C16" s="1">
+        <f>SUM(C4:C14)</f>
         <v>50</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated week 1 notes and lab instructions
</commit_message>
<xml_diff>
--- a/Labs/Lab01/Lab1Rubric_CS295N.xlsx
+++ b/Labs/Lab01/Lab1Rubric_CS295N.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birdb/Projects/CS295N-CourseMaterials/Labs/Lab01/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CS295N-CourseMaterials/Labs/Lab01/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84504B0D-85CC-E646-B0D8-7688CAD1FCBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{51AACEAF-2105-2648-9516-24FEB16F2DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24520" yWindow="2100" windowWidth="12320" windowHeight="15760" activeTab="1" xr2:uid="{E89A4641-8758-0A47-BBA8-AF46CE147EE8}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14540" xr2:uid="{E89A4641-8758-0A47-BBA8-AF46CE147EE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
   <si>
     <t>Lab 1</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>Here's the grade breakdown:</t>
+  </si>
+  <si>
+    <t>Lab 1 Grading Rubric</t>
   </si>
 </sst>
 </file>
@@ -173,9 +176,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -213,7 +216,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -319,7 +322,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -461,7 +464,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -471,8 +474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{281C4FE9-3D20-9541-ADFE-932BAB85A5E5}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B17"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection sqref="A1:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -482,7 +485,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -598,7 +601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4A17B91-A5F8-5746-983D-59BEC50C3108}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>

</xml_diff>